<commit_message>
Urkunde für die Jüngste Gruppe
</commit_message>
<xml_diff>
--- a/BWB-Auswertung/Resources/Vorlagen/Auswertungsbogen.xlsx
+++ b/BWB-Auswertung/Resources/Vorlagen/Auswertungsbogen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maximilian.janzen\source\repos\jf-bundeswettbewerb\BWB-Auswertung\BWB-Auswertung\Resources\Vorlagen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maximilian.janzen\source\repos\jf-bundeswettbewerbPublic\BWB-Auswertung\Resources\Vorlagen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7497C450-4B7F-46DF-8087-5E6B6CB43C99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01883173-72D7-4A88-AE7C-5FA134E60627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -835,6 +835,261 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="4"/>
+    </xf>
+    <xf numFmtId="2" fontId="21" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="21" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="9" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="9" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="9" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="18"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="18"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="18"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="3" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="3" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="3" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="7"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="7"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="7"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="21" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="9"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="9"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="9"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -843,261 +1098,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="9"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="9"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="9"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="7"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="7"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="7"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="2" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="2" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="18"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="18"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="18"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="165" fontId="21" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="3" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="3" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="3" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="4"/>
-    </xf>
-    <xf numFmtId="2" fontId="21" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="21" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="9" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="9" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="9" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1139,7 +1139,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="7667" y="9428288"/>
+          <a:off x="5762" y="9441623"/>
           <a:ext cx="2722245" cy="12065"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="2722245" cy="12065"/>
@@ -1360,9 +1360,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1400,9 +1400,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1435,26 +1435,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1487,26 +1470,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1683,107 +1649,106 @@
   <dimension ref="A1:O39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19:J19"/>
+      <selection activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.33203125" customWidth="1"/>
     <col min="2" max="2" width="4.6640625" customWidth="1"/>
     <col min="3" max="3" width="8" customWidth="1"/>
     <col min="4" max="4" width="4.6640625" customWidth="1"/>
-    <col min="5" max="5" width="6.88671875" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="7" width="4.6640625" customWidth="1"/>
-    <col min="8" max="8" width="6.88671875" customWidth="1"/>
+    <col min="7" max="7" width="5" customWidth="1"/>
+    <col min="8" max="8" width="6.83203125" customWidth="1"/>
     <col min="9" max="9" width="4.6640625" customWidth="1"/>
     <col min="10" max="10" width="17.33203125" customWidth="1"/>
     <col min="11" max="11" width="3.33203125" customWidth="1"/>
-    <col min="12" max="12" width="10.44140625" customWidth="1"/>
+    <col min="12" max="12" width="10.5" customWidth="1"/>
     <col min="13" max="13" width="4.6640625" customWidth="1"/>
-    <col min="14" max="14" width="9.33203125" customWidth="1"/>
-    <col min="15" max="15" width="10.44140625" customWidth="1"/>
+    <col min="14" max="15" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-    </row>
-    <row r="2" spans="1:15" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+    <row r="1" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="106" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="106"/>
+      <c r="C1" s="106"/>
+      <c r="D1" s="106"/>
+      <c r="E1" s="106"/>
+      <c r="F1" s="106"/>
+      <c r="G1" s="106"/>
+      <c r="H1" s="106"/>
+      <c r="I1" s="106"/>
+      <c r="J1" s="106"/>
+      <c r="K1" s="106"/>
+      <c r="L1" s="106"/>
+      <c r="M1" s="106"/>
+      <c r="N1" s="106"/>
+      <c r="O1" s="106"/>
+    </row>
+    <row r="2" spans="1:15" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="107" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="27" t="s">
+      <c r="B2" s="108"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="101"/>
+      <c r="H2" s="101"/>
+      <c r="I2" s="101"/>
+      <c r="J2" s="102"/>
+      <c r="K2" s="98" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="28"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="30"/>
+      <c r="L2" s="99"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="37"/>
       <c r="O2" s="2"/>
     </row>
-    <row r="3" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+    <row r="3" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="98" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="27" t="s">
+      <c r="B3" s="99"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="101"/>
+      <c r="G3" s="101"/>
+      <c r="H3" s="101"/>
+      <c r="I3" s="101"/>
+      <c r="J3" s="102"/>
+      <c r="K3" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="28"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="30"/>
+      <c r="L3" s="99"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="37"/>
       <c r="O3" s="2"/>
     </row>
-    <row r="4" spans="1:15" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="31"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="32"/>
-      <c r="K4" s="32"/>
-      <c r="L4" s="32"/>
-      <c r="M4" s="32"/>
-      <c r="N4" s="33"/>
+    <row r="4" spans="1:15" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="103"/>
+      <c r="B4" s="104"/>
+      <c r="C4" s="104"/>
+      <c r="D4" s="104"/>
+      <c r="E4" s="104"/>
+      <c r="F4" s="104"/>
+      <c r="G4" s="104"/>
+      <c r="H4" s="104"/>
+      <c r="I4" s="104"/>
+      <c r="J4" s="104"/>
+      <c r="K4" s="104"/>
+      <c r="L4" s="104"/>
+      <c r="M4" s="104"/>
+      <c r="N4" s="105"/>
       <c r="O4" s="2"/>
     </row>
-    <row r="5" spans="1:15" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -1800,26 +1765,26 @@
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
     </row>
-    <row r="6" spans="1:15" ht="25.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="34" t="s">
+    <row r="6" spans="1:15" ht="25.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="35"/>
-      <c r="L6" s="35"/>
-      <c r="M6" s="35"/>
-      <c r="N6" s="36"/>
+      <c r="B6" s="96"/>
+      <c r="C6" s="96"/>
+      <c r="D6" s="96"/>
+      <c r="E6" s="96"/>
+      <c r="F6" s="96"/>
+      <c r="G6" s="96"/>
+      <c r="H6" s="96"/>
+      <c r="I6" s="96"/>
+      <c r="J6" s="96"/>
+      <c r="K6" s="96"/>
+      <c r="L6" s="96"/>
+      <c r="M6" s="96"/>
+      <c r="N6" s="97"/>
       <c r="O6" s="2"/>
     </row>
-    <row r="7" spans="1:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -1836,179 +1801,179 @@
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
     </row>
-    <row r="8" spans="1:15" ht="18.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="37" t="s">
+    <row r="8" spans="1:15" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="38"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="43" t="s">
+      <c r="B8" s="63"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="63"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="44"/>
-      <c r="I8" s="44"/>
-      <c r="J8" s="45"/>
-      <c r="K8" s="46">
+      <c r="H8" s="69"/>
+      <c r="I8" s="69"/>
+      <c r="J8" s="70"/>
+      <c r="K8" s="71">
         <v>1000</v>
       </c>
-      <c r="L8" s="47"/>
-      <c r="M8" s="48" t="s">
+      <c r="L8" s="72"/>
+      <c r="M8" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="N8" s="49"/>
+      <c r="N8" s="74"/>
       <c r="O8" s="2"/>
     </row>
-    <row r="9" spans="1:15" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="40"/>
-      <c r="B9" s="41"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="52" t="s">
+    <row r="9" spans="1:15" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="65"/>
+      <c r="B9" s="66"/>
+      <c r="C9" s="66"/>
+      <c r="D9" s="66"/>
+      <c r="E9" s="66"/>
+      <c r="F9" s="67"/>
+      <c r="G9" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="53"/>
-      <c r="I9" s="54"/>
+      <c r="H9" s="78"/>
+      <c r="I9" s="79"/>
       <c r="J9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K9" s="55"/>
-      <c r="L9" s="56"/>
-      <c r="M9" s="50"/>
-      <c r="N9" s="51"/>
+      <c r="K9" s="80"/>
+      <c r="L9" s="81"/>
+      <c r="M9" s="75"/>
+      <c r="N9" s="76"/>
       <c r="O9" s="2"/>
     </row>
-    <row r="10" spans="1:15" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="61" t="s">
+    <row r="10" spans="1:15" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="62"/>
-      <c r="C10" s="62"/>
-      <c r="D10" s="62"/>
-      <c r="E10" s="62"/>
-      <c r="F10" s="63"/>
-      <c r="G10" s="29">
+      <c r="B10" s="59"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="35">
         <v>1</v>
       </c>
-      <c r="H10" s="64"/>
-      <c r="I10" s="30"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="37"/>
       <c r="J10" s="1">
         <v>0</v>
       </c>
-      <c r="K10" s="57"/>
-      <c r="L10" s="58"/>
-      <c r="M10" s="55"/>
-      <c r="N10" s="56"/>
+      <c r="K10" s="82"/>
+      <c r="L10" s="83"/>
+      <c r="M10" s="80"/>
+      <c r="N10" s="81"/>
       <c r="O10" s="2"/>
     </row>
-    <row r="11" spans="1:15" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="65" t="s">
+    <row r="11" spans="1:15" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="89" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="62"/>
-      <c r="C11" s="62"/>
-      <c r="D11" s="62"/>
-      <c r="E11" s="62"/>
-      <c r="F11" s="63"/>
-      <c r="G11" s="29">
+      <c r="B11" s="59"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="35">
         <v>1</v>
       </c>
-      <c r="H11" s="64"/>
-      <c r="I11" s="30"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="37"/>
       <c r="J11" s="1">
         <v>0</v>
       </c>
-      <c r="K11" s="57"/>
-      <c r="L11" s="58"/>
-      <c r="M11" s="57"/>
-      <c r="N11" s="58"/>
+      <c r="K11" s="82"/>
+      <c r="L11" s="83"/>
+      <c r="M11" s="82"/>
+      <c r="N11" s="83"/>
       <c r="O11" s="2"/>
     </row>
-    <row r="12" spans="1:15" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="61" t="s">
+    <row r="12" spans="1:15" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="62"/>
-      <c r="C12" s="62"/>
-      <c r="D12" s="62"/>
-      <c r="E12" s="62"/>
-      <c r="F12" s="63"/>
-      <c r="G12" s="29">
+      <c r="B12" s="59"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="59"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="35">
         <v>1</v>
       </c>
-      <c r="H12" s="64"/>
-      <c r="I12" s="30"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="37"/>
       <c r="J12" s="1">
         <v>0</v>
       </c>
-      <c r="K12" s="57"/>
-      <c r="L12" s="58"/>
-      <c r="M12" s="57"/>
-      <c r="N12" s="58"/>
+      <c r="K12" s="82"/>
+      <c r="L12" s="83"/>
+      <c r="M12" s="82"/>
+      <c r="N12" s="83"/>
       <c r="O12" s="2"/>
     </row>
-    <row r="13" spans="1:15" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="61" t="s">
+    <row r="13" spans="1:15" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="62"/>
-      <c r="C13" s="62"/>
-      <c r="D13" s="62"/>
-      <c r="E13" s="62"/>
-      <c r="F13" s="63"/>
-      <c r="G13" s="29">
+      <c r="B13" s="59"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="59"/>
+      <c r="F13" s="60"/>
+      <c r="G13" s="35">
         <v>1</v>
       </c>
-      <c r="H13" s="64"/>
-      <c r="I13" s="30"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="37"/>
       <c r="J13" s="1">
         <v>0</v>
       </c>
-      <c r="K13" s="57"/>
-      <c r="L13" s="58"/>
-      <c r="M13" s="57"/>
-      <c r="N13" s="58"/>
+      <c r="K13" s="82"/>
+      <c r="L13" s="83"/>
+      <c r="M13" s="82"/>
+      <c r="N13" s="83"/>
       <c r="O13" s="2"/>
     </row>
-    <row r="14" spans="1:15" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="61" t="s">
+    <row r="14" spans="1:15" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="62"/>
-      <c r="C14" s="62"/>
-      <c r="D14" s="62"/>
-      <c r="E14" s="62"/>
-      <c r="F14" s="63"/>
-      <c r="G14" s="29">
+      <c r="B14" s="59"/>
+      <c r="C14" s="59"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="59"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="35">
         <v>1</v>
       </c>
-      <c r="H14" s="64"/>
-      <c r="I14" s="30"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="37"/>
       <c r="J14" s="1">
         <v>0</v>
       </c>
-      <c r="K14" s="59"/>
-      <c r="L14" s="60"/>
-      <c r="M14" s="57"/>
-      <c r="N14" s="58"/>
+      <c r="K14" s="84"/>
+      <c r="L14" s="85"/>
+      <c r="M14" s="82"/>
+      <c r="N14" s="83"/>
       <c r="O14" s="2"/>
     </row>
-    <row r="15" spans="1:15" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="66" t="s">
+    <row r="15" spans="1:15" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="67"/>
-      <c r="C15" s="67"/>
-      <c r="D15" s="67"/>
-      <c r="E15" s="67"/>
-      <c r="F15" s="67"/>
-      <c r="G15" s="67"/>
-      <c r="H15" s="67"/>
-      <c r="I15" s="68"/>
+      <c r="B15" s="49"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="49"/>
+      <c r="H15" s="49"/>
+      <c r="I15" s="50"/>
       <c r="J15" s="1">
         <f>SUM(J10:J14)</f>
         <v>0</v>
@@ -2020,23 +1985,23 @@
         <f>J15</f>
         <v>0</v>
       </c>
-      <c r="M15" s="57"/>
-      <c r="N15" s="58"/>
+      <c r="M15" s="82"/>
+      <c r="N15" s="83"/>
       <c r="O15" s="2"/>
     </row>
-    <row r="16" spans="1:15" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="65" t="s">
+    <row r="16" spans="1:15" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="89" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="69"/>
-      <c r="C16" s="69"/>
-      <c r="D16" s="70">
+      <c r="B16" s="90"/>
+      <c r="C16" s="90"/>
+      <c r="D16" s="94">
         <f>I16/86400</f>
         <v>1.1574074074074073E-5</v>
       </c>
-      <c r="E16" s="70"/>
-      <c r="F16" s="70"/>
-      <c r="G16" s="70"/>
+      <c r="E16" s="94"/>
+      <c r="F16" s="94"/>
+      <c r="G16" s="94"/>
       <c r="H16" s="13" t="s">
         <v>43</v>
       </c>
@@ -2046,55 +2011,55 @@
       <c r="J16" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="K16" s="71"/>
-      <c r="L16" s="72"/>
-      <c r="M16" s="57"/>
-      <c r="N16" s="58"/>
+      <c r="K16" s="51"/>
+      <c r="L16" s="52"/>
+      <c r="M16" s="82"/>
+      <c r="N16" s="83"/>
       <c r="O16" s="2"/>
     </row>
-    <row r="17" spans="1:15" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="78"/>
-      <c r="C17" s="78"/>
+      <c r="B17" s="93"/>
+      <c r="C17" s="93"/>
       <c r="D17" s="14"/>
-      <c r="E17" s="73" t="s">
+      <c r="E17" s="86" t="s">
         <v>39</v>
       </c>
-      <c r="F17" s="74"/>
-      <c r="G17" s="74"/>
-      <c r="H17" s="74"/>
-      <c r="I17" s="74"/>
-      <c r="J17" s="75"/>
+      <c r="F17" s="87"/>
+      <c r="G17" s="87"/>
+      <c r="H17" s="87"/>
+      <c r="I17" s="87"/>
+      <c r="J17" s="88"/>
       <c r="K17" s="5" t="s">
         <v>15</v>
       </c>
       <c r="L17" s="6">
         <v>0</v>
       </c>
-      <c r="M17" s="57"/>
-      <c r="N17" s="58"/>
+      <c r="M17" s="82"/>
+      <c r="N17" s="83"/>
       <c r="O17" s="2"/>
     </row>
-    <row r="18" spans="1:15" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="65" t="s">
+    <row r="18" spans="1:15" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="89" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="69"/>
-      <c r="C18" s="69"/>
-      <c r="D18" s="76" t="s">
+      <c r="B18" s="90"/>
+      <c r="C18" s="90"/>
+      <c r="D18" s="91" t="s">
         <v>16</v>
       </c>
-      <c r="E18" s="76"/>
+      <c r="E18" s="91"/>
       <c r="F18" s="12">
         <v>0</v>
       </c>
-      <c r="G18" s="77" t="s">
+      <c r="G18" s="92" t="s">
         <v>41</v>
       </c>
-      <c r="H18" s="77"/>
-      <c r="I18" s="108">
+      <c r="H18" s="92"/>
+      <c r="I18" s="21">
         <v>1</v>
       </c>
       <c r="J18" s="16" t="s">
@@ -2106,35 +2071,35 @@
       <c r="L18" s="6">
         <v>0</v>
       </c>
-      <c r="M18" s="59"/>
-      <c r="N18" s="60"/>
+      <c r="M18" s="84"/>
+      <c r="N18" s="85"/>
       <c r="O18" s="2"/>
     </row>
-    <row r="19" spans="1:15" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="79"/>
-      <c r="B19" s="79"/>
-      <c r="C19" s="79"/>
-      <c r="D19" s="79"/>
-      <c r="E19" s="79"/>
-      <c r="F19" s="79"/>
-      <c r="G19" s="80"/>
-      <c r="H19" s="81" t="s">
+    <row r="19" spans="1:15" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="I19" s="82"/>
-      <c r="J19" s="83"/>
+      <c r="I19" s="25"/>
+      <c r="J19" s="26"/>
       <c r="K19" s="7"/>
       <c r="L19" s="8">
         <v>0</v>
       </c>
-      <c r="M19" s="84">
+      <c r="M19" s="61">
         <f>L19</f>
         <v>0</v>
       </c>
-      <c r="N19" s="85"/>
+      <c r="N19" s="57"/>
       <c r="O19" s="2"/>
     </row>
-    <row r="20" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -2151,271 +2116,271 @@
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
     </row>
-    <row r="21" spans="1:15" ht="18.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="37" t="s">
+    <row r="21" spans="1:15" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="38"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="38"/>
-      <c r="F21" s="39"/>
-      <c r="G21" s="43" t="s">
+      <c r="B21" s="63"/>
+      <c r="C21" s="63"/>
+      <c r="D21" s="63"/>
+      <c r="E21" s="63"/>
+      <c r="F21" s="64"/>
+      <c r="G21" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="H21" s="44"/>
-      <c r="I21" s="44"/>
-      <c r="J21" s="45"/>
-      <c r="K21" s="46">
+      <c r="H21" s="69"/>
+      <c r="I21" s="69"/>
+      <c r="J21" s="70"/>
+      <c r="K21" s="71">
         <v>400</v>
       </c>
-      <c r="L21" s="47"/>
-      <c r="M21" s="48" t="s">
+      <c r="L21" s="72"/>
+      <c r="M21" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="N21" s="49"/>
+      <c r="N21" s="74"/>
       <c r="O21" s="2"/>
     </row>
-    <row r="22" spans="1:15" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="40"/>
-      <c r="B22" s="41"/>
-      <c r="C22" s="41"/>
-      <c r="D22" s="41"/>
-      <c r="E22" s="41"/>
-      <c r="F22" s="42"/>
-      <c r="G22" s="52" t="s">
+    <row r="22" spans="1:15" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="65"/>
+      <c r="B22" s="66"/>
+      <c r="C22" s="66"/>
+      <c r="D22" s="66"/>
+      <c r="E22" s="66"/>
+      <c r="F22" s="67"/>
+      <c r="G22" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="H22" s="53"/>
-      <c r="I22" s="54"/>
+      <c r="H22" s="78"/>
+      <c r="I22" s="79"/>
       <c r="J22" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K22" s="55"/>
-      <c r="L22" s="56"/>
-      <c r="M22" s="50"/>
-      <c r="N22" s="51"/>
+      <c r="K22" s="80"/>
+      <c r="L22" s="81"/>
+      <c r="M22" s="75"/>
+      <c r="N22" s="76"/>
       <c r="O22" s="2"/>
     </row>
-    <row r="23" spans="1:15" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="61" t="s">
+    <row r="23" spans="1:15" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="62"/>
-      <c r="C23" s="62"/>
-      <c r="D23" s="62"/>
-      <c r="E23" s="62"/>
-      <c r="F23" s="63"/>
-      <c r="G23" s="29">
+      <c r="B23" s="59"/>
+      <c r="C23" s="59"/>
+      <c r="D23" s="59"/>
+      <c r="E23" s="59"/>
+      <c r="F23" s="60"/>
+      <c r="G23" s="35">
         <v>1</v>
       </c>
-      <c r="H23" s="64"/>
-      <c r="I23" s="30"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="37"/>
       <c r="J23" s="1">
         <v>0</v>
       </c>
-      <c r="K23" s="57"/>
-      <c r="L23" s="58"/>
-      <c r="M23" s="55"/>
-      <c r="N23" s="56"/>
+      <c r="K23" s="82"/>
+      <c r="L23" s="83"/>
+      <c r="M23" s="80"/>
+      <c r="N23" s="81"/>
       <c r="O23" s="2"/>
     </row>
-    <row r="24" spans="1:15" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="61" t="s">
+    <row r="24" spans="1:15" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="62"/>
-      <c r="C24" s="62"/>
-      <c r="D24" s="62"/>
-      <c r="E24" s="62"/>
-      <c r="F24" s="63"/>
-      <c r="G24" s="29">
+      <c r="B24" s="59"/>
+      <c r="C24" s="59"/>
+      <c r="D24" s="59"/>
+      <c r="E24" s="59"/>
+      <c r="F24" s="60"/>
+      <c r="G24" s="35">
         <v>1</v>
       </c>
-      <c r="H24" s="64"/>
-      <c r="I24" s="30"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="37"/>
       <c r="J24" s="1">
         <v>0</v>
       </c>
-      <c r="K24" s="57"/>
-      <c r="L24" s="58"/>
-      <c r="M24" s="57"/>
-      <c r="N24" s="58"/>
+      <c r="K24" s="82"/>
+      <c r="L24" s="83"/>
+      <c r="M24" s="82"/>
+      <c r="N24" s="83"/>
       <c r="O24" s="2"/>
     </row>
-    <row r="25" spans="1:15" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="61" t="s">
+    <row r="25" spans="1:15" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="62"/>
-      <c r="C25" s="62"/>
-      <c r="D25" s="62"/>
-      <c r="E25" s="62"/>
-      <c r="F25" s="63"/>
-      <c r="G25" s="29">
+      <c r="B25" s="59"/>
+      <c r="C25" s="59"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="59"/>
+      <c r="F25" s="60"/>
+      <c r="G25" s="35">
         <v>1</v>
       </c>
-      <c r="H25" s="64"/>
-      <c r="I25" s="30"/>
+      <c r="H25" s="36"/>
+      <c r="I25" s="37"/>
       <c r="J25" s="1">
         <v>0</v>
       </c>
-      <c r="K25" s="57"/>
-      <c r="L25" s="58"/>
-      <c r="M25" s="57"/>
-      <c r="N25" s="58"/>
+      <c r="K25" s="82"/>
+      <c r="L25" s="83"/>
+      <c r="M25" s="82"/>
+      <c r="N25" s="83"/>
       <c r="O25" s="2"/>
     </row>
-    <row r="26" spans="1:15" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="61" t="s">
+    <row r="26" spans="1:15" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="62"/>
-      <c r="C26" s="62"/>
-      <c r="D26" s="62"/>
-      <c r="E26" s="62"/>
-      <c r="F26" s="63"/>
-      <c r="G26" s="29">
+      <c r="B26" s="59"/>
+      <c r="C26" s="59"/>
+      <c r="D26" s="59"/>
+      <c r="E26" s="59"/>
+      <c r="F26" s="60"/>
+      <c r="G26" s="35">
         <v>1</v>
       </c>
-      <c r="H26" s="64"/>
-      <c r="I26" s="30"/>
+      <c r="H26" s="36"/>
+      <c r="I26" s="37"/>
       <c r="J26" s="1">
         <v>0</v>
       </c>
-      <c r="K26" s="57"/>
-      <c r="L26" s="58"/>
-      <c r="M26" s="57"/>
-      <c r="N26" s="58"/>
+      <c r="K26" s="82"/>
+      <c r="L26" s="83"/>
+      <c r="M26" s="82"/>
+      <c r="N26" s="83"/>
       <c r="O26" s="2"/>
     </row>
-    <row r="27" spans="1:15" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="61" t="s">
+    <row r="27" spans="1:15" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="62"/>
-      <c r="C27" s="62"/>
-      <c r="D27" s="62"/>
-      <c r="E27" s="62"/>
-      <c r="F27" s="63"/>
-      <c r="G27" s="29">
+      <c r="B27" s="59"/>
+      <c r="C27" s="59"/>
+      <c r="D27" s="59"/>
+      <c r="E27" s="59"/>
+      <c r="F27" s="60"/>
+      <c r="G27" s="35">
         <v>1</v>
       </c>
-      <c r="H27" s="64"/>
-      <c r="I27" s="30"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="37"/>
       <c r="J27" s="1">
         <v>0</v>
       </c>
-      <c r="K27" s="57"/>
-      <c r="L27" s="58"/>
-      <c r="M27" s="57"/>
-      <c r="N27" s="58"/>
+      <c r="K27" s="82"/>
+      <c r="L27" s="83"/>
+      <c r="M27" s="82"/>
+      <c r="N27" s="83"/>
       <c r="O27" s="2"/>
     </row>
-    <row r="28" spans="1:15" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="61" t="s">
+    <row r="28" spans="1:15" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="62"/>
-      <c r="C28" s="62"/>
-      <c r="D28" s="62"/>
-      <c r="E28" s="62"/>
-      <c r="F28" s="63"/>
-      <c r="G28" s="29">
+      <c r="B28" s="59"/>
+      <c r="C28" s="59"/>
+      <c r="D28" s="59"/>
+      <c r="E28" s="59"/>
+      <c r="F28" s="60"/>
+      <c r="G28" s="35">
         <v>1</v>
       </c>
-      <c r="H28" s="64"/>
-      <c r="I28" s="30"/>
+      <c r="H28" s="36"/>
+      <c r="I28" s="37"/>
       <c r="J28" s="1">
         <v>0</v>
       </c>
-      <c r="K28" s="57"/>
-      <c r="L28" s="58"/>
-      <c r="M28" s="57"/>
-      <c r="N28" s="58"/>
+      <c r="K28" s="82"/>
+      <c r="L28" s="83"/>
+      <c r="M28" s="82"/>
+      <c r="N28" s="83"/>
       <c r="O28" s="2"/>
     </row>
-    <row r="29" spans="1:15" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="61" t="s">
+    <row r="29" spans="1:15" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="62"/>
-      <c r="C29" s="62"/>
-      <c r="D29" s="62"/>
-      <c r="E29" s="62"/>
-      <c r="F29" s="63"/>
-      <c r="G29" s="29">
+      <c r="B29" s="59"/>
+      <c r="C29" s="59"/>
+      <c r="D29" s="59"/>
+      <c r="E29" s="59"/>
+      <c r="F29" s="60"/>
+      <c r="G29" s="35">
         <v>1</v>
       </c>
-      <c r="H29" s="64"/>
-      <c r="I29" s="30"/>
+      <c r="H29" s="36"/>
+      <c r="I29" s="37"/>
       <c r="J29" s="1">
         <v>0</v>
       </c>
-      <c r="K29" s="57"/>
-      <c r="L29" s="58"/>
-      <c r="M29" s="57"/>
-      <c r="N29" s="58"/>
+      <c r="K29" s="82"/>
+      <c r="L29" s="83"/>
+      <c r="M29" s="82"/>
+      <c r="N29" s="83"/>
       <c r="O29" s="2"/>
     </row>
-    <row r="30" spans="1:15" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="61" t="s">
+    <row r="30" spans="1:15" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="62"/>
-      <c r="C30" s="62"/>
-      <c r="D30" s="62"/>
-      <c r="E30" s="62"/>
-      <c r="F30" s="63"/>
-      <c r="G30" s="29">
+      <c r="B30" s="59"/>
+      <c r="C30" s="59"/>
+      <c r="D30" s="59"/>
+      <c r="E30" s="59"/>
+      <c r="F30" s="60"/>
+      <c r="G30" s="35">
         <v>1</v>
       </c>
-      <c r="H30" s="64"/>
-      <c r="I30" s="30"/>
+      <c r="H30" s="36"/>
+      <c r="I30" s="37"/>
       <c r="J30" s="1">
         <v>0</v>
       </c>
-      <c r="K30" s="57"/>
-      <c r="L30" s="58"/>
-      <c r="M30" s="57"/>
-      <c r="N30" s="58"/>
+      <c r="K30" s="82"/>
+      <c r="L30" s="83"/>
+      <c r="M30" s="82"/>
+      <c r="N30" s="83"/>
       <c r="O30" s="2"/>
     </row>
-    <row r="31" spans="1:15" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="61" t="s">
+    <row r="31" spans="1:15" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="62"/>
-      <c r="C31" s="62"/>
-      <c r="D31" s="62"/>
-      <c r="E31" s="62"/>
-      <c r="F31" s="63"/>
-      <c r="G31" s="29">
+      <c r="B31" s="59"/>
+      <c r="C31" s="59"/>
+      <c r="D31" s="59"/>
+      <c r="E31" s="59"/>
+      <c r="F31" s="60"/>
+      <c r="G31" s="35">
         <v>1</v>
       </c>
-      <c r="H31" s="64"/>
-      <c r="I31" s="30"/>
+      <c r="H31" s="36"/>
+      <c r="I31" s="37"/>
       <c r="J31" s="1">
         <v>0</v>
       </c>
-      <c r="K31" s="59"/>
-      <c r="L31" s="60"/>
-      <c r="M31" s="57"/>
-      <c r="N31" s="58"/>
+      <c r="K31" s="84"/>
+      <c r="L31" s="85"/>
+      <c r="M31" s="82"/>
+      <c r="N31" s="83"/>
       <c r="O31" s="2"/>
     </row>
-    <row r="32" spans="1:15" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="66" t="s">
+    <row r="32" spans="1:15" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="B32" s="67"/>
-      <c r="C32" s="67"/>
-      <c r="D32" s="67"/>
-      <c r="E32" s="67"/>
-      <c r="F32" s="67"/>
-      <c r="G32" s="67"/>
-      <c r="H32" s="67"/>
-      <c r="I32" s="68"/>
+      <c r="B32" s="49"/>
+      <c r="C32" s="49"/>
+      <c r="D32" s="49"/>
+      <c r="E32" s="49"/>
+      <c r="F32" s="49"/>
+      <c r="G32" s="49"/>
+      <c r="H32" s="49"/>
+      <c r="I32" s="50"/>
       <c r="J32" s="1">
         <f>SUM(J23:J31)</f>
         <v>0</v>
@@ -2427,82 +2392,82 @@
         <f>J32</f>
         <v>0</v>
       </c>
-      <c r="M32" s="57"/>
-      <c r="N32" s="58"/>
+      <c r="M32" s="82"/>
+      <c r="N32" s="83"/>
       <c r="O32" s="2"/>
     </row>
-    <row r="33" spans="1:15" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B33" s="89">
+      <c r="B33" s="29">
         <f>G33/86400</f>
         <v>1.1574074074074073E-5</v>
       </c>
-      <c r="C33" s="89"/>
-      <c r="D33" s="89"/>
-      <c r="E33" s="89"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
       <c r="F33" s="19" t="s">
         <v>43</v>
       </c>
       <c r="G33" s="18">
         <v>1</v>
       </c>
-      <c r="H33" s="86" t="s">
+      <c r="H33" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="I33" s="87"/>
-      <c r="J33" s="88"/>
-      <c r="K33" s="71"/>
-      <c r="L33" s="72"/>
-      <c r="M33" s="57"/>
-      <c r="N33" s="58"/>
+      <c r="I33" s="54"/>
+      <c r="J33" s="55"/>
+      <c r="K33" s="51"/>
+      <c r="L33" s="52"/>
+      <c r="M33" s="82"/>
+      <c r="N33" s="83"/>
       <c r="O33" s="2"/>
     </row>
-    <row r="34" spans="1:15" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B34" s="89">
+      <c r="B34" s="29">
         <f>G34/86400</f>
         <v>1.1574074074074073E-5</v>
       </c>
-      <c r="C34" s="89"/>
-      <c r="D34" s="89"/>
-      <c r="E34" s="89"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="29"/>
       <c r="F34" s="19" t="s">
         <v>43</v>
       </c>
       <c r="G34" s="20">
         <v>1</v>
       </c>
-      <c r="H34" s="91" t="s">
+      <c r="H34" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="I34" s="91"/>
-      <c r="J34" s="92"/>
-      <c r="K34" s="90">
+      <c r="I34" s="27"/>
+      <c r="J34" s="28"/>
+      <c r="K34" s="56">
         <f>G34-G33</f>
         <v>0</v>
       </c>
-      <c r="L34" s="85"/>
-      <c r="M34" s="59"/>
-      <c r="N34" s="60"/>
+      <c r="L34" s="57"/>
+      <c r="M34" s="84"/>
+      <c r="N34" s="85"/>
       <c r="O34" s="2"/>
     </row>
-    <row r="35" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="79"/>
-      <c r="B35" s="79"/>
-      <c r="C35" s="79"/>
-      <c r="D35" s="79"/>
-      <c r="E35" s="79"/>
-      <c r="F35" s="79"/>
-      <c r="G35" s="80"/>
-      <c r="H35" s="81" t="s">
+    <row r="35" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="22"/>
+      <c r="B35" s="22"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="23"/>
+      <c r="H35" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="I35" s="82"/>
-      <c r="J35" s="83"/>
+      <c r="I35" s="25"/>
+      <c r="J35" s="26"/>
       <c r="K35" s="7"/>
       <c r="L35" s="8">
         <v>0</v>
@@ -2516,7 +2481,7 @@
       </c>
       <c r="O35" s="2"/>
     </row>
-    <row r="36" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -2533,103 +2498,111 @@
       <c r="N36" s="2"/>
       <c r="O36" s="2"/>
     </row>
-    <row r="37" spans="1:15" ht="29.55" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="95" t="s">
+    <row r="37" spans="1:15" ht="29.65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="B37" s="96"/>
-      <c r="C37" s="96"/>
-      <c r="D37" s="96"/>
-      <c r="E37" s="96"/>
-      <c r="F37" s="97"/>
-      <c r="G37" s="29">
+      <c r="B37" s="33"/>
+      <c r="C37" s="33"/>
+      <c r="D37" s="33"/>
+      <c r="E37" s="33"/>
+      <c r="F37" s="34"/>
+      <c r="G37" s="35">
         <f>SUM(G10:I14)+SUM(G23:I31)</f>
         <v>14</v>
       </c>
-      <c r="H37" s="64"/>
-      <c r="I37" s="30"/>
-      <c r="J37" s="98" t="s">
+      <c r="H37" s="36"/>
+      <c r="I37" s="37"/>
+      <c r="J37" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="K37" s="99"/>
-      <c r="L37" s="100"/>
-      <c r="M37" s="101">
-        <f>G37/14</f>
+      <c r="K37" s="39"/>
+      <c r="L37" s="40"/>
+      <c r="M37" s="41">
         <v>1</v>
       </c>
-      <c r="N37" s="102"/>
+      <c r="N37" s="42"/>
       <c r="O37" s="11"/>
     </row>
-    <row r="38" spans="1:15" ht="29.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="103" t="s">
+    <row r="38" spans="1:15" ht="29.65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="B38" s="103"/>
-      <c r="C38" s="103"/>
-      <c r="D38" s="103"/>
-      <c r="E38" s="103"/>
-      <c r="F38" s="103"/>
-      <c r="G38" s="103"/>
-      <c r="H38" s="103"/>
-      <c r="I38" s="103"/>
-      <c r="J38" s="104"/>
-      <c r="K38" s="105">
-        <v>0</v>
-      </c>
-      <c r="L38" s="106"/>
-      <c r="M38" s="106"/>
-      <c r="N38" s="107"/>
+      <c r="B38" s="43"/>
+      <c r="C38" s="43"/>
+      <c r="D38" s="43"/>
+      <c r="E38" s="43"/>
+      <c r="F38" s="43"/>
+      <c r="G38" s="43"/>
+      <c r="H38" s="43"/>
+      <c r="I38" s="43"/>
+      <c r="J38" s="44"/>
+      <c r="K38" s="45">
+        <v>0</v>
+      </c>
+      <c r="L38" s="46"/>
+      <c r="M38" s="46"/>
+      <c r="N38" s="47"/>
       <c r="O38" s="11"/>
     </row>
-    <row r="39" spans="1:15" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="93" t="s">
+    <row r="39" spans="1:15" ht="37.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="B39" s="94"/>
-      <c r="C39" s="94"/>
-      <c r="D39" s="94"/>
-      <c r="E39" s="94"/>
-      <c r="F39" s="94"/>
-      <c r="G39" s="94"/>
-      <c r="H39" s="94"/>
-      <c r="I39" s="94"/>
-      <c r="J39" s="94"/>
-      <c r="K39" s="94"/>
-      <c r="L39" s="94"/>
-      <c r="M39" s="94"/>
-      <c r="N39" s="94"/>
-      <c r="O39" s="94"/>
+      <c r="B39" s="31"/>
+      <c r="C39" s="31"/>
+      <c r="D39" s="31"/>
+      <c r="E39" s="31"/>
+      <c r="F39" s="31"/>
+      <c r="G39" s="31"/>
+      <c r="H39" s="31"/>
+      <c r="I39" s="31"/>
+      <c r="J39" s="31"/>
+      <c r="K39" s="31"/>
+      <c r="L39" s="31"/>
+      <c r="M39" s="31"/>
+      <c r="N39" s="31"/>
+      <c r="O39" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="81">
-    <mergeCell ref="A35:G35"/>
-    <mergeCell ref="H35:J35"/>
-    <mergeCell ref="H34:J34"/>
-    <mergeCell ref="B34:E34"/>
-    <mergeCell ref="A39:O39"/>
-    <mergeCell ref="A37:F37"/>
-    <mergeCell ref="G37:I37"/>
-    <mergeCell ref="J37:L37"/>
-    <mergeCell ref="M37:N37"/>
-    <mergeCell ref="A38:J38"/>
-    <mergeCell ref="K38:N38"/>
-    <mergeCell ref="A32:I32"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="H33:J33"/>
-    <mergeCell ref="B33:E33"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="A29:F29"/>
-    <mergeCell ref="G29:I29"/>
-    <mergeCell ref="A30:F30"/>
-    <mergeCell ref="G30:I30"/>
-    <mergeCell ref="A31:F31"/>
-    <mergeCell ref="G31:I31"/>
-    <mergeCell ref="A26:F26"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="A27:F27"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="A28:F28"/>
-    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="A4:N4"/>
+    <mergeCell ref="A6:N6"/>
+    <mergeCell ref="A8:F9"/>
+    <mergeCell ref="G8:J8"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="M8:N9"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="K9:L14"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="M10:N18"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="A14:F14"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="E17:J17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="B17:C17"/>
     <mergeCell ref="A19:G19"/>
     <mergeCell ref="H19:J19"/>
     <mergeCell ref="M19:N19"/>
@@ -2646,43 +2619,34 @@
     <mergeCell ref="G24:I24"/>
     <mergeCell ref="A25:F25"/>
     <mergeCell ref="G25:I25"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="E17:J17"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="A14:F14"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="A15:I15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="A6:N6"/>
-    <mergeCell ref="A8:F9"/>
-    <mergeCell ref="G8:J8"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="M8:N9"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="K9:L14"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="M10:N18"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="A12:F12"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="A13:F13"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="A4:N4"/>
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A26:F26"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="A27:F27"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="A28:F28"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="A29:F29"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="A30:F30"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="G31:I31"/>
+    <mergeCell ref="A32:I32"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="H33:J33"/>
+    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="A35:G35"/>
+    <mergeCell ref="H35:J35"/>
+    <mergeCell ref="H34:J34"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="A39:O39"/>
+    <mergeCell ref="A37:F37"/>
+    <mergeCell ref="G37:I37"/>
+    <mergeCell ref="J37:L37"/>
+    <mergeCell ref="M37:N37"/>
+    <mergeCell ref="A38:J38"/>
+    <mergeCell ref="K38:N38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>